<commit_message>
feat: re-integrate WBS advanced features (KPIs, Baselines, Budget/Resource roll-up)
</commit_message>
<xml_diff>
--- a/public/project_template.xlsx
+++ b/public/project_template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Projects" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Goals" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Scopes" state="visible" r:id="rId6"/>
+    <sheet sheetId="2" name="Final Products" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Phases" state="visible" r:id="rId6"/>
     <sheet sheetId="4" name="Deliverables" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Work Packages" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -64,13 +65,16 @@
     <t>Budget</t>
   </si>
   <si>
-    <t>Goal Description</t>
+    <t>Final Product Description</t>
   </si>
   <si>
     <t>Timeline</t>
   </si>
   <si>
-    <t>Scope Description(s)</t>
+    <t>Phase Description</t>
+  </si>
+  <si>
+    <t>Deliverable Description</t>
   </si>
   <si>
     <t>Assignee</t>
@@ -590,16 +594,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="50" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -607,15 +611,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update excel templates and sample data with timeline columns
</commit_message>
<xml_diff>
--- a/public/project_template.xlsx
+++ b/public/project_template.xlsx
@@ -1,113 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
   <sheets>
-    <sheet sheetId="1" name="Projects" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Final Products" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Phases" state="visible" r:id="rId6"/>
-    <sheet sheetId="4" name="Deliverables" state="visible" r:id="rId7"/>
-    <sheet sheetId="5" name="Work Packages" state="visible" r:id="rId8"/>
+    <sheet name="Projects" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Products" sheetId="2" r:id="rId2"/>
+    <sheet name="Phases" sheetId="3" r:id="rId3"/>
+    <sheet name="Deliverables" sheetId="4" r:id="rId4"/>
+    <sheet name="Work Packages" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>BusinessUnit</t>
-  </si>
-  <si>
-    <t>Budget Plan</t>
-  </si>
-  <si>
-    <t>Budget Actual</t>
-  </si>
-  <si>
-    <t>Budget Additional</t>
-  </si>
-  <si>
-    <t>Vendor Name</t>
-  </si>
-  <si>
-    <t>Vendor Contact</t>
-  </si>
-  <si>
-    <t>Vendor Value</t>
-  </si>
-  <si>
-    <t>Man Days Plan</t>
-  </si>
-  <si>
-    <t>Man Days Actual</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Budget</t>
-  </si>
-  <si>
-    <t>Final Product Description</t>
-  </si>
-  <si>
-    <t>Timeline</t>
-  </si>
-  <si>
-    <t>Phase Description</t>
-  </si>
-  <si>
-    <t>Deliverable Description</t>
-  </si>
-  <si>
-    <t>Assignee</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,23 +68,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -463,199 +400,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="9" width="15" customWidth="1"/>
-    <col min="10" max="11" width="20" customWidth="1"/>
-    <col min="12" max="14" width="15" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Owner</v>
+      </c>
+      <c r="D1" t="str">
+        <v>PM</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="F1" t="str">
+        <v>BusinessUnit</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Budget Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Budget Actual</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Budget Additional</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Vendor Name</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Vendor Contact</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Vendor Value</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Man Days Plan</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Man Days Actual</v>
+      </c>
+      <c r="O1" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="P1" t="str">
+        <v>End Date</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>Actual Start Date</v>
+      </c>
+      <c r="R1" t="str">
+        <v>Actual End Date</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:R1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Project Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Owner</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Budget</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="F1" t="str">
+        <v>End Date</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Actual Start Date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Actual End Date</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Final Product Description</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Owner</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Budget</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Timeline</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="G1" t="str">
+        <v>End Date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Actual Start Date</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Actual End Date</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Phase Description</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Owner</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Budget</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="G1" t="str">
+        <v>End Date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Actual Start Date</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Actual End Date</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="2" width="50" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-  </cols>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Deliverable Description</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Assignee</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Budget</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Start Date</v>
+      </c>
+      <c r="G1" t="str">
+        <v>End Date</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Actual Start Date</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Actual End Date</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: KPI Management, Import/Export, and Analytics Year Filter
</commit_message>
<xml_diff>
--- a/public/project_template.xlsx
+++ b/public/project_template.xlsx
@@ -1,59 +1,135 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011" filterPrivacy="true"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Projects" sheetId="1" r:id="rId1"/>
-    <sheet name="Final Products" sheetId="2" r:id="rId2"/>
-    <sheet name="Phases" sheetId="3" r:id="rId3"/>
-    <sheet name="Deliverables" sheetId="4" r:id="rId4"/>
-    <sheet name="Work Packages" sheetId="5" r:id="rId5"/>
+    <sheet sheetId="1" name="Projects" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Final Products" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="Phases" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="Deliverables" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="Work Packages" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="KPIs" state="visible" r:id="rId9"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>BusinessUnit</t>
+  </si>
+  <si>
+    <t>Budget Plan</t>
+  </si>
+  <si>
+    <t>Budget Actual</t>
+  </si>
+  <si>
+    <t>Budget Additional</t>
+  </si>
+  <si>
+    <t>Vendor Name</t>
+  </si>
+  <si>
+    <t>Vendor Contact</t>
+  </si>
+  <si>
+    <t>Vendor Value</t>
+  </si>
+  <si>
+    <t>Man Days Plan</t>
+  </si>
+  <si>
+    <t>Man Days Actual</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Final Product Description</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Phase Description</t>
+  </si>
+  <si>
+    <t>Deliverable Description</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Entity Type</t>
+  </si>
+  <si>
+    <t>Entity Name</t>
+  </si>
+  <si>
+    <t>Entity ID</t>
+  </si>
+  <si>
+    <t>KPI Name</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,14 +144,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -400,240 +485,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="9" width="15" customWidth="1"/>
+    <col min="10" max="11" width="20" customWidth="1"/>
+    <col min="12" max="14" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Owner</v>
-      </c>
-      <c r="D1" t="str">
-        <v>PM</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BusinessUnit</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Budget Plan</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Budget Actual</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Budget Additional</v>
-      </c>
-      <c r="J1" t="str">
-        <v>Vendor Name</v>
-      </c>
-      <c r="K1" t="str">
-        <v>Vendor Contact</v>
-      </c>
-      <c r="L1" t="str">
-        <v>Vendor Value</v>
-      </c>
-      <c r="M1" t="str">
-        <v>Man Days Plan</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Man Days Actual</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="P1" t="str">
-        <v>End Date</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>Actual Start Date</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Actual End Date</v>
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Project Name</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Owner</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Budget</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="F1" t="str">
-        <v>End Date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>Actual Start Date</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Actual End Date</v>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Final Product Description</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Owner</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Budget</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Timeline</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>End Date</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Actual Start Date</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Actual End Date</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Phase Description</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Owner</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Budget</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>End Date</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Actual Start Date</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Actual End Date</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Deliverable Description</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="C1" t="str">
-        <v>Assignee</v>
-      </c>
-      <c r="D1" t="str">
-        <v>Budget</v>
-      </c>
-      <c r="E1" t="str">
-        <v>Status</v>
-      </c>
-      <c r="F1" t="str">
-        <v>Start Date</v>
-      </c>
-      <c r="G1" t="str">
-        <v>End Date</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Actual Start Date</v>
-      </c>
-      <c r="I1" t="str">
-        <v>Actual End Date</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
-  </ignoredErrors>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>